<commit_message>
Agile crm testcase updation
</commit_message>
<xml_diff>
--- a/AgileCRM_FT_01.xlsx
+++ b/AgileCRM_FT_01.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\parag\Desktop\Virajm\test cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2520337D-FF51-496F-BEB1-FDDC44E8B603}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5E37BE0-DC25-4368-879D-E7CD1EC6A6A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{18718D20-C006-4A04-A538-0B6C8EDA0DD4}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="120">
   <si>
     <t>Orange_HRMS</t>
   </si>
@@ -76,32 +76,6 @@
   </si>
   <si>
     <t>Module Name</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Add New Contact and verifying it should displayed into </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>contacts</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> tab</t>
-    </r>
   </si>
   <si>
     <t>Contacts</t>
@@ -273,17 +247,11 @@
     <t>Delete Contact and verify that it should get remove from contact list</t>
   </si>
   <si>
-    <t>AJC_AC_01</t>
-  </si>
-  <si>
     <t>1. Delete Alert Window should be displayed
 2.Contact should get remove from contact list</t>
   </si>
   <si>
     <t>Deals</t>
-  </si>
-  <si>
-    <t>AJC_AD_01</t>
   </si>
   <si>
     <t>Add New Deal and verifying it should displayed into Deals list</t>
@@ -320,25 +288,7 @@
 3.Click on save button</t>
   </si>
   <si>
-    <t>AJC_DD_02</t>
-  </si>
-  <si>
-    <t>AJC_EC_02</t>
-  </si>
-  <si>
-    <t>AJC_DC_03</t>
-  </si>
-  <si>
-    <t>Delete Deal and verify that it should get deleted from deals list</t>
-  </si>
-  <si>
     <t xml:space="preserve">Delete contact from contacts list </t>
-  </si>
-  <si>
-    <t>Delete deal from New Deals list</t>
-  </si>
-  <si>
-    <t>Deal should be deleted from deals list</t>
   </si>
   <si>
     <t>New added contact should be displayed into contacts page.</t>
@@ -389,9 +339,6 @@
       </rPr>
       <t xml:space="preserve"> Window should be displayed</t>
     </r>
-  </si>
-  <si>
-    <t>AJC_ED_02</t>
   </si>
   <si>
     <t>Edit the Name of the Deal</t>
@@ -401,9 +348,6 @@
 2.Click on the deal.
 3.Click Edit deal button
 4.Edit the name and click on Update button</t>
-  </si>
-  <si>
-    <t>name-Chitale Bandhu</t>
   </si>
   <si>
     <t>1.Click on Deals Tab
@@ -482,6 +426,342 @@
   </si>
   <si>
     <t>change existing deal from new to Lost milestone</t>
+  </si>
+  <si>
+    <t>Delete Contact and verify that it should dispalyed in Trash.</t>
+  </si>
+  <si>
+    <t>1.Click on the ellipsis menu of contact
+2.Click on delete option 
+3.click on yes button.
+4.click on Trash tab and click on contacts tab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Delete Alert Window should be displayed
+2.Contact should get remove from contact list
+3. Deleted contact should displayed in trash </t>
+  </si>
+  <si>
+    <t>1.name-Chitale Bandhu</t>
+  </si>
+  <si>
+    <t>Add deal with invalid details</t>
+  </si>
+  <si>
+    <t>1.Click on Deals Tab
+2.Click on Add deals button
+3.Enter details and do not select any milestone.
+4.Click on save button</t>
+  </si>
+  <si>
+    <t>1.1234
+value-ABCD</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1."</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="5"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please enter a valid number</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" validation message should be highlighted below value Textfield 
+2. "</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="5"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>This field is required.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" validation message should be highlited below milestone dropdown.</t>
+    </r>
+  </si>
+  <si>
+    <t>Delete Deal from Deals</t>
+  </si>
+  <si>
+    <t>Add New Contact and verifying it should displayed into contacts tab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Delete deal by drag and drop from Deals list </t>
+  </si>
+  <si>
+    <t>1.Click on Deals Tab
+2.Click and hold on the deal and drag and release at delete option.
+3.Click on yes button</t>
+  </si>
+  <si>
+    <r>
+      <t>1.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="5"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Are you sure you want to delete? </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Window should be displayed.
+2.Deal should be deleted from deals list</t>
+    </r>
+  </si>
+  <si>
+    <t>Companies</t>
+  </si>
+  <si>
+    <t>AJC_AddConatct_01</t>
+  </si>
+  <si>
+    <t>AJC_EditContact_02</t>
+  </si>
+  <si>
+    <t>AJC_DeleteContact_03</t>
+  </si>
+  <si>
+    <t>AJC_AddDeal_01</t>
+  </si>
+  <si>
+    <t>AJC_EditDeal_02</t>
+  </si>
+  <si>
+    <t>AJC_DeleteDeal_03</t>
+  </si>
+  <si>
+    <t>AJC_AddCompany_04</t>
+  </si>
+  <si>
+    <t>Add company with details</t>
+  </si>
+  <si>
+    <t>Add company with valid details</t>
+  </si>
+  <si>
+    <t>1. Click on companies tab
+2.Click on Add Company button
+3. Enter all details and click on save button</t>
+  </si>
+  <si>
+    <t>1.Name- OlaCabs
+ url- www.olacabs.com</t>
+  </si>
+  <si>
+    <r>
+      <t>1.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="5"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">New Company </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Window should be dispalyed.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+2.Company timeline page should be displayed. </t>
+    </r>
+  </si>
+  <si>
+    <t>Add company with same details already exist</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="5"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Company name already exists.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="5"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Validation mesaage should be displayed.</t>
+    </r>
+  </si>
+  <si>
+    <t>Add company with null details</t>
+  </si>
+  <si>
+    <r>
+      <t>"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="5"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>This field is required.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" validation message should be dispalyed below Name textfield</t>
+    </r>
+  </si>
+  <si>
+    <t>AJC_EditCompany_04</t>
+  </si>
+  <si>
+    <t>Edit company details</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Edit company details </t>
+  </si>
+  <si>
+    <t>1. Click on companies tab
+2.Click on the company name
+3. edit Name of company and click on update button</t>
+  </si>
+  <si>
+    <t>Name-Swiggy</t>
+  </si>
+  <si>
+    <t>Company name should be updated</t>
+  </si>
+  <si>
+    <t>update of the company details</t>
+  </si>
+  <si>
+    <t>1. Click on companies tab
+2.Click on the company name
+3. Enter phone No and select country from dropdown of company and click on update button</t>
+  </si>
+  <si>
+    <t>phone no-889988997
+contry-india</t>
+  </si>
+  <si>
+    <t>Company details should be updated</t>
+  </si>
+  <si>
+    <t>AJC_DeleteCompany_04</t>
+  </si>
+  <si>
+    <t>Delete company from companies</t>
+  </si>
+  <si>
+    <t>Delete company from companies list</t>
+  </si>
+  <si>
+    <t>1. Click on companies tab
+2.Select the checkbox of company and click on delete button</t>
+  </si>
+  <si>
+    <t>Company should be deleted from list</t>
+  </si>
+  <si>
+    <t>Delete company from companies list and verify it should displayed into Trash</t>
+  </si>
+  <si>
+    <t>1. Click on companies tab
+2.Select the checkbox of company and click on delete button
+3.Click on Trash tab and click on companies tab</t>
+  </si>
+  <si>
+    <t>Deleted company should be listed into trash</t>
   </si>
 </sst>
 </file>
@@ -491,7 +771,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -503,14 +783,6 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -533,6 +805,25 @@
     <font>
       <sz val="11"/>
       <color theme="5" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="5"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -637,15 +928,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -654,10 +945,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -675,6 +966,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -696,8 +990,8 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1014,16 +1308,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97179EE3-9AD8-4826-8058-8249CAFC12FE}">
-  <dimension ref="A1:K27"/>
+  <dimension ref="A1:K32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="6.33203125" customWidth="1"/>
-    <col min="2" max="3" width="15.77734375" customWidth="1"/>
+    <col min="2" max="2" width="15.77734375" customWidth="1"/>
+    <col min="3" max="3" width="25" customWidth="1"/>
     <col min="4" max="4" width="30.77734375" customWidth="1"/>
     <col min="5" max="5" width="15.77734375" customWidth="1"/>
     <col min="6" max="6" width="32.5546875" customWidth="1"/>
@@ -1034,52 +1329,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="18" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="15"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="16"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
     </row>
     <row r="2" spans="1:11" ht="18" x14ac:dyDescent="0.3">
-      <c r="A2" s="16">
+      <c r="A2" s="17">
         <v>44730</v>
       </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="18"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="19"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
     </row>
     <row r="3" spans="1:11" ht="18" x14ac:dyDescent="0.3">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="15"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="16"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
     </row>
     <row r="4" spans="1:11" ht="18" x14ac:dyDescent="0.3">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="19"/>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
@@ -1125,46 +1420,46 @@
         <v>1</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>40</v>
+        <v>14</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>86</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>14</v>
+        <v>81</v>
       </c>
       <c r="E6" s="9">
         <v>1</v>
       </c>
       <c r="F6" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="H6" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="G6" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="H6" s="8" t="s">
-        <v>19</v>
-      </c>
       <c r="I6" s="8" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="115.2" x14ac:dyDescent="0.3">
       <c r="E7" s="9">
-        <f t="shared" ref="E7:E17" si="0">E6+0.1</f>
+        <f t="shared" ref="E7:E21" si="0">E6+0.1</f>
         <v>1.1000000000000001</v>
       </c>
       <c r="F7" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="H7" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="G7" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="H7" s="8" t="s">
-        <v>21</v>
-      </c>
       <c r="I7" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
@@ -1173,16 +1468,16 @@
         <v>1.2000000000000002</v>
       </c>
       <c r="F8" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="H8" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="I8" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="G8" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="H8" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
@@ -1191,40 +1486,40 @@
         <v>1.3000000000000003</v>
       </c>
       <c r="F9" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="H9" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="G9" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="H9" s="8" t="s">
+      <c r="I9" s="10" t="s">
         <v>29</v>
-      </c>
-      <c r="I9" s="10" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="C10" s="4" t="s">
-        <v>53</v>
+        <v>87</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E10" s="9">
         <f t="shared" si="0"/>
         <v>1.4000000000000004</v>
       </c>
       <c r="F10" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="G10" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="H10" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G10" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="H10" s="5" t="s">
+      <c r="I10" s="10" t="s">
         <v>26</v>
-      </c>
-      <c r="I10" s="10" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
@@ -1233,244 +1528,442 @@
         <v>1.5000000000000004</v>
       </c>
       <c r="F11" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="G11" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="G11" s="12" t="s">
-        <v>36</v>
-      </c>
       <c r="H11" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="C12" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>39</v>
+        <v>88</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>49</v>
       </c>
       <c r="E12" s="9">
         <f t="shared" si="0"/>
         <v>1.6000000000000005</v>
       </c>
-      <c r="F12" s="10" t="s">
-        <v>56</v>
+      <c r="F12" s="8" t="s">
+        <v>38</v>
       </c>
       <c r="G12" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H12" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I12" s="10" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A13" s="5">
-        <v>2</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="D13" s="10" t="s">
-        <v>44</v>
-      </c>
+      <c r="C13" s="4"/>
+      <c r="D13" s="10"/>
       <c r="E13" s="9">
         <f t="shared" si="0"/>
         <v>1.7000000000000006</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>45</v>
+        <v>72</v>
       </c>
       <c r="G13" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>47</v>
+        <v>73</v>
+      </c>
+      <c r="H13" s="11" t="s">
+        <v>16</v>
       </c>
       <c r="I13" s="10" t="s">
-        <v>48</v>
+        <v>74</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A14" s="5">
+        <v>2</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>41</v>
+      </c>
       <c r="E14" s="9">
         <f t="shared" si="0"/>
         <v>1.8000000000000007</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="G14" s="12" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+      <c r="I14" s="10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
       <c r="E15" s="9">
         <f t="shared" si="0"/>
         <v>1.9000000000000008</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="G15" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="E16" s="13">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F16" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="G16" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="H16" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="I16" s="10" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="E17" s="13">
+        <f>E16+0.01</f>
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="F17" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="G17" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="H17" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="D18" s="1"/>
+      <c r="E18" s="13">
+        <f t="shared" ref="E18:E20" si="1">E17+0.01</f>
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="F18" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="G18" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="H15" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="D16" s="1"/>
-      <c r="E16" s="20">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="F16" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="G16" s="12" t="s">
+      <c r="H18" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="I18" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="E19" s="13">
+        <f t="shared" si="1"/>
+        <v>1.1300000000000001</v>
+      </c>
+      <c r="F19" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="G19" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="H19" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="I19" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="E20" s="13">
+        <f t="shared" si="1"/>
+        <v>1.1400000000000001</v>
+      </c>
+      <c r="F20" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="G20" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="H20" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="I20" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="E21" s="13">
+        <f>E20+0.01</f>
+        <v>1.1500000000000001</v>
+      </c>
+      <c r="F21" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="G21" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="H21" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="I21" s="10" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+      <c r="C22" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="E22" s="9">
+        <v>2.1</v>
+      </c>
+      <c r="F22" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="G22" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="H16" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="I16" s="5" t="s">
+      <c r="H22" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="I22" s="10" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+      <c r="E23" s="9">
+        <f>E22+0.1</f>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F23" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="G23" s="12" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="17" spans="3:9" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="E17" s="20">
-        <v>1.1100000000000001</v>
-      </c>
-      <c r="F17" s="10" t="s">
+      <c r="H23" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="I23" s="10" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="E24" s="9">
+        <f t="shared" ref="E24:E25" si="2">E23+0.1</f>
+        <v>2.3000000000000003</v>
+      </c>
+      <c r="F24" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="G24" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="H24" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="I24" s="10" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="C25" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="D25" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="G17" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="H17" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="I17" s="5" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="18" spans="3:9" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="E18" s="20">
-        <v>1.1200000000000001</v>
-      </c>
-      <c r="F18" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="G18" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="H18" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="I18" s="5" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="19" spans="3:9" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="E19" s="20">
-        <v>1.1299999999999999</v>
-      </c>
-      <c r="F19" s="10" t="s">
+      <c r="E25" s="9">
+        <f t="shared" si="2"/>
+        <v>2.4000000000000004</v>
+      </c>
+      <c r="F25" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="G19" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="H19" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="I19" s="10" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="20" spans="3:9" ht="72" x14ac:dyDescent="0.3">
-      <c r="C20" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="E20" s="9">
-        <v>2.1</v>
-      </c>
-      <c r="F20" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="G20" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="H20" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="I20" s="10" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="21" spans="3:9" ht="72" x14ac:dyDescent="0.3">
-      <c r="F21" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="G21" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="H21" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="I21" s="10" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="22" spans="3:9" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="F22" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="G22" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="H22" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="I22" s="10" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="27" spans="3:9" ht="72" x14ac:dyDescent="0.3">
-      <c r="C27" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="D27" s="10" t="s">
-        <v>55</v>
-      </c>
+      <c r="G25" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="H25" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="I25" s="12" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A26" s="4">
+        <v>3</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="E26" s="9">
+        <v>3</v>
+      </c>
+      <c r="F26" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="G26" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="H26" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="I26" s="12" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="E27" s="9">
-        <f>E15+0.1</f>
-        <v>2.0000000000000009</v>
+        <f>E26+0.1</f>
+        <v>3.1</v>
       </c>
       <c r="F27" s="10" t="s">
-        <v>57</v>
+        <v>98</v>
       </c>
       <c r="G27" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="H27" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="I27" s="12" t="s">
-        <v>58</v>
+        <v>95</v>
+      </c>
+      <c r="H27" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="I27" s="21" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="E28" s="9">
+        <f>E27+0.1</f>
+        <v>3.2</v>
+      </c>
+      <c r="F28" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="G28" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="H28" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="I28" s="12" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="C29" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="E29" s="9">
+        <f>E28+0.1</f>
+        <v>3.3000000000000003</v>
+      </c>
+      <c r="F29" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="G29" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="H29" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="I29" s="12" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="E30" s="9">
+        <f t="shared" ref="E30:E31" si="3">E29+0.1</f>
+        <v>3.4000000000000004</v>
+      </c>
+      <c r="F30" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="G30" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="H30" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="I30" s="12" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="C31" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="E31" s="9">
+        <f t="shared" si="3"/>
+        <v>3.5000000000000004</v>
+      </c>
+      <c r="F31" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="G31" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="H31" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="I31" s="12" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+      <c r="E32" s="9">
+        <f>E31+0.1</f>
+        <v>3.6000000000000005</v>
+      </c>
+      <c r="F32" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="G32" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="H32" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="I32" s="12" t="s">
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -1480,6 +1973,7 @@
     <mergeCell ref="A3:E3"/>
     <mergeCell ref="A4:E4"/>
   </mergeCells>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
AgileCrm test case updation
</commit_message>
<xml_diff>
--- a/AgileCRM_FT_01.xlsx
+++ b/AgileCRM_FT_01.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\parag\Desktop\Virajm\test cases\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AutomationProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5E37BE0-DC25-4368-879D-E7CD1EC6A6A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B311C526-0236-457C-8261-715B66A76890}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{18718D20-C006-4A04-A538-0B6C8EDA0DD4}"/>
   </bookViews>
@@ -761,7 +761,7 @@
 3.Click on Trash tab and click on companies tab</t>
   </si>
   <si>
-    <t>Deleted company should be listed into trash</t>
+    <t>Deleted company should be listed into trash.</t>
   </si>
 </sst>
 </file>
@@ -969,6 +969,9 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -988,9 +991,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1310,8 +1310,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97179EE3-9AD8-4826-8058-8249CAFC12FE}">
   <dimension ref="A1:K32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="I33" sqref="I33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1329,52 +1329,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="18" x14ac:dyDescent="0.3">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="16"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="17"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
     </row>
     <row r="2" spans="1:11" ht="18" x14ac:dyDescent="0.3">
-      <c r="A2" s="17">
+      <c r="A2" s="18">
         <v>44730</v>
       </c>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="19"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="20"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
     </row>
     <row r="3" spans="1:11" ht="18" x14ac:dyDescent="0.3">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="15"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="16"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="17"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
     </row>
     <row r="4" spans="1:11" ht="18" x14ac:dyDescent="0.3">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="20"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
+      <c r="B4" s="21"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
@@ -1446,7 +1446,7 @@
     </row>
     <row r="7" spans="1:11" ht="115.2" x14ac:dyDescent="0.3">
       <c r="E7" s="9">
-        <f t="shared" ref="E7:E21" si="0">E6+0.1</f>
+        <f t="shared" ref="E7:E15" si="0">E6+0.1</f>
         <v>1.1000000000000001</v>
       </c>
       <c r="F7" s="10" t="s">
@@ -1860,7 +1860,7 @@
       <c r="H27" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="I27" s="21" t="s">
+      <c r="I27" s="14" t="s">
         <v>99</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated TestCases of agileCrm
</commit_message>
<xml_diff>
--- a/AgileCRM_FT_01.xlsx
+++ b/AgileCRM_FT_01.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AutomationProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B311C526-0236-457C-8261-715B66A76890}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC24DE0D-F757-4C3F-8602-17EC114AB2F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{18718D20-C006-4A04-A538-0B6C8EDA0DD4}"/>
   </bookViews>
@@ -1310,8 +1310,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97179EE3-9AD8-4826-8058-8249CAFC12FE}">
   <dimension ref="A1:K32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="I33" sqref="I33"/>
+    <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>